<commit_message>
updated Excel upload template file
</commit_message>
<xml_diff>
--- a/public/MagIC/help/TemplateForMagICDataUpload.xlsx
+++ b/public/MagIC/help/TemplateForMagICDataUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njarboe/git/earthref/MagIC/public/MagIC/help/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njarboe/Dropbox/MagIC/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6A7B6A-6D6B-9C4F-A9FB-7D0502EA0191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6770E9D0-AEF2-5B4C-9A40-2245E3E033DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="4340" windowWidth="40660" windowHeight="17560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35620" yWindow="18160" windowWidth="28800" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="103">
   <si>
     <t>location</t>
   </si>
@@ -319,17 +319,38 @@
     <t>u= unknown or s=standard (calibration) measurement</t>
   </si>
   <si>
-    <t>dir_tilt_correction</t>
-  </si>
-  <si>
-    <t>Use 0 for geographic and 100 for straigraphic correction. See online data model (earthref.org/MagIC/data-models/3.0) for more options</t>
+    <t>tab delimited</t>
+  </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>sites</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>specimens</t>
+  </si>
+  <si>
+    <t>measurements</t>
+  </si>
+  <si>
+    <t>criteria</t>
+  </si>
+  <si>
+    <t>ages</t>
+  </si>
+  <si>
+    <t>images</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +445,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -450,7 +478,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -459,11 +487,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -749,9 +776,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -783,79 +810,87 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T3" s="7" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9C34F620-28DD-584C-81E7-7005AEAE7241}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{446F0401-45C5-6A45-86FC-B28AF52A05B1}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{E96087E6-3612-CB44-9987-3C7711184554}"/>
-    <hyperlink ref="O2" r:id="rId4" xr:uid="{23D353E8-954C-544B-A7BB-B9C72C378727}"/>
-    <hyperlink ref="P2" r:id="rId5" xr:uid="{67A62DCE-2283-234B-AD9C-E102A35B29CE}"/>
-    <hyperlink ref="Q2" r:id="rId6" xr:uid="{CCEF7671-6222-114A-9977-FCF80F12A0F2}"/>
-    <hyperlink ref="R2" r:id="rId7" xr:uid="{4FAFED3C-50B5-5048-BF14-1B5F7B457148}"/>
-    <hyperlink ref="S2" r:id="rId8" xr:uid="{93B82F0D-35CE-404F-8AA8-454E6308443F}"/>
-    <hyperlink ref="M2" r:id="rId9" xr:uid="{2674D4CC-35D4-1847-B325-D51AC3116BD8}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{9C34F620-28DD-584C-81E7-7005AEAE7241}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{446F0401-45C5-6A45-86FC-B28AF52A05B1}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{E96087E6-3612-CB44-9987-3C7711184554}"/>
+    <hyperlink ref="O3" r:id="rId4" xr:uid="{23D353E8-954C-544B-A7BB-B9C72C378727}"/>
+    <hyperlink ref="P3" r:id="rId5" xr:uid="{67A62DCE-2283-234B-AD9C-E102A35B29CE}"/>
+    <hyperlink ref="Q3" r:id="rId6" xr:uid="{CCEF7671-6222-114A-9977-FCF80F12A0F2}"/>
+    <hyperlink ref="R3" r:id="rId7" xr:uid="{4FAFED3C-50B5-5048-BF14-1B5F7B457148}"/>
+    <hyperlink ref="S3" r:id="rId8" xr:uid="{93B82F0D-35CE-404F-8AA8-454E6308443F}"/>
+    <hyperlink ref="M3" r:id="rId9" xr:uid="{2674D4CC-35D4-1847-B325-D51AC3116BD8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -864,10 +899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,113 +910,114 @@
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" customWidth="1"/>
-    <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="18.1640625" customWidth="1"/>
-    <col min="21" max="21" width="12.5" customWidth="1"/>
-    <col min="22" max="22" width="6.1640625" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" customWidth="1"/>
-    <col min="27" max="27" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" customWidth="1"/>
+    <col min="20" max="20" width="12.5" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" customWidth="1"/>
+    <col min="26" max="26" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
-      <c r="R1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P3" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q3" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="S2" s="8" t="s">
+      <c r="R3" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="S3" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="T3" t="s">
         <v>35</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="U3" t="s">
         <v>36</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="V3" t="s">
         <v>37</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="W3" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="X3" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="Z3" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E806FDCE-A996-9740-992F-ADA9B1F4CC28}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{946ECC33-6397-0F4E-A9DF-4370EA562670}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{56583B7E-F643-2745-BD6D-74D3AC45133F}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{A1ACE978-A1A9-7247-97B3-79C6EE3E96CF}"/>
-    <hyperlink ref="M2" r:id="rId5" xr:uid="{D4B2482E-89C5-7B41-8349-F7A1F0AC2D43}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{E806FDCE-A996-9740-992F-ADA9B1F4CC28}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{946ECC33-6397-0F4E-A9DF-4370EA562670}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{56583B7E-F643-2745-BD6D-74D3AC45133F}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{A1ACE978-A1A9-7247-97B3-79C6EE3E96CF}"/>
+    <hyperlink ref="M3" r:id="rId5" xr:uid="{D4B2482E-89C5-7B41-8349-F7A1F0AC2D43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -990,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D31" sqref="D30:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,45 +1037,71 @@
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{DAFE0553-C6F4-7640-BB8C-254BE913163E}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{DAFE0553-C6F4-7640-BB8C-254BE913163E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1047,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,49 +1121,75 @@
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7A2EDDE2-F721-764A-B4FC-A7FF1A78C260}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{7A2EDDE2-F721-764A-B4FC-A7FF1A78C260}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1109,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1195,83 +1283,109 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X4" s="5" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{D9599BEB-D39E-E94A-A11B-EECB49B8CECA}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{D9599BEB-D39E-E94A-A11B-EECB49B8CECA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1279,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1292,34 +1406,60 @@
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F3" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A6D71CDD-3B29-6946-82EA-0BEAB50A3F4D}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{A6D71CDD-3B29-6946-82EA-0BEAB50A3F4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1327,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1480,7 @@
     <col min="10" max="10" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1351,47 +1491,73 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L3" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{FEDEE117-2269-304D-B46F-F57EDE9FE2DD}"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{FEDEE117-2269-304D-B46F-F57EDE9FE2DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1399,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,28 +1576,54 @@
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F3" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>